<commit_message>
add blurb column to db
</commit_message>
<xml_diff>
--- a/wp_news_articles_3.xlsx
+++ b/wp_news_articles_3.xlsx
@@ -1620,7 +1620,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ &quot;00:00:00&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1694,14 +1694,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2009,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>